<commit_message>
Update Bill of Material Summary.xlsx
</commit_message>
<xml_diff>
--- a/build/bom/Bill of Material Summary.xlsx
+++ b/build/bom/Bill of Material Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\ergo kb\BlueJay\github\BlueJay\build\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6A3E6D-F0AC-4C6B-9D64-31CE5BB038D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DFF400-E9B2-4F52-8F7A-CF35C7111572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6705" yWindow="2985" windowWidth="28800" windowHeight="15885" xr2:uid="{9EA9E6DC-B467-4955-8A4C-EEF6BFEE18C3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Ref</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Molex 0548190519 Mini USB receptacle</t>
-  </si>
-  <si>
-    <t>Mil-Max sockets</t>
   </si>
   <si>
     <t>switch puller</t>
@@ -573,7 +570,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B21" sqref="B21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +702,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,7 +716,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,7 +730,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,7 +744,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,7 +814,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,15 +836,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f>2*B20</f>
-        <v>108</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
@@ -865,22 +853,22 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>